<commit_message>
Enhance examples and configuration handling: update README for clarity on statement configurations, streamline demo scripts to utilize built-in configurations, and ensure consistent formatting and linting across all modified files.
</commit_message>
<xml_diff>
--- a/examples/scripts/output/financial_statements.xlsx/test_statement.xlsx
+++ b/examples/scripts/output/financial_statements.xlsx/test_statement.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,370 +473,814 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total Current Assets</t>
+          <t xml:space="preserve">  Cash &amp; Equivalents</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>current_assets_subtotal</t>
+          <t>cash_and_equivalents</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>50</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>50</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>167</t>
+          <t>55</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>186</t>
+          <t>61</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>207</t>
+          <t>67</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total Assets</t>
+          <t xml:space="preserve">  Accounts Receivable</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>total_assets</t>
+          <t>accounts_receivable</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>100</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>100</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>482</t>
+          <t>112</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>517</t>
+          <t>125</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>554</t>
+          <t>140</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total Liabilities</t>
+          <t xml:space="preserve">  Total Current Assets</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>total_liabilities</t>
+          <t>total_current_assets</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>150</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>150</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>239</t>
+          <t>167</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>186</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>260</t>
+          <t>207</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Retained Earnings</t>
+          <t xml:space="preserve">  Property, Plant &amp; Equipment</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>retained_earnings</t>
+          <t>property_plant_equipment</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1,305</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2,500</t>
+          <t>300</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3,912</t>
+          <t>315</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>5,558</t>
+          <t>331</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>7,543</t>
+          <t>347</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total Equity</t>
+          <t xml:space="preserve">  Total Assets</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>total_equity</t>
+          <t>total_assets</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1,405</t>
+          <t>450</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2,600</t>
+          <t>450</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>4,012</t>
+          <t>482</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>5,658</t>
+          <t>517</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>7,643</t>
+          <t>554</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total Liabilities &amp; Equity</t>
+          <t xml:space="preserve">  Accounts Payable</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>total_liabs_equity</t>
+          <t>accounts_payable</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1,635</t>
+          <t>80</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2,830</t>
+          <t>80</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>4,251</t>
+          <t>86</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>5,908</t>
+          <t>93</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>7,903</t>
+          <t>101</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Gross Profit</t>
+          <t xml:space="preserve">  Total Debt</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>gross_profit</t>
+          <t>total_debt</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1,400</t>
+          <t>150</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1,700</t>
+          <t>150</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1,945</t>
+          <t>153</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2,233</t>
+          <t>156</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2,574</t>
+          <t>159</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Total Operating Expenses</t>
+          <t xml:space="preserve">  Total Liabilities</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>total_operating_expenses</t>
+          <t>total_liabilities</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>330</t>
+          <t>230</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>405</t>
+          <t>230</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>405</t>
+          <t>239</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>426</t>
+          <t>249</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>439</t>
+          <t>260</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Operating Income</t>
+          <t xml:space="preserve">  Common Stock</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>operating_income</t>
+          <t>common_stock</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1,070</t>
+          <t>100</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1,295</t>
+          <t>100</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1,540</t>
+          <t>100</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>1,808</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2,134</t>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t xml:space="preserve">  Prior Retained Earnings</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>prior_retained_earnings</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Dividends</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>dividends</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>-10</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>-10</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>-10</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Total Equity</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>total_equity</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1,735</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>3,005</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>4,416</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>6,084</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>8,082</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Total Liabilities &amp; Equity</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>total_liabilities_equity</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1,965</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>3,235</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>4,656</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>6,333</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>8,342</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Revenue</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>revenue</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1,000</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1,200</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>1,320</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>1,452</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1,597</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Cost of Goods Sold</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>cost_of_goods_sold</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>-400</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>-500</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-625</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>-781</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>-977</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Gross Profit</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>gross_profit</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1,400</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1,700</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1,945</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2,233</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2,574</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Operating Expenses</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>operating_expenses</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>-100</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>-120</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>-130</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>-137</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-158</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Operating Income</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>operating_income</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1,500</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>1,820</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2,075</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2,371</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2,732</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Interest Expense</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>interest_expense</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>-50</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>-60</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-63</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-66</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>-69</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Income Before Tax</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>income_before_tax</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1,550</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>1,880</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2,138</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2,437</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2,801</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Income Tax</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>income_tax</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>-75</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>-90</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>-108</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>-130</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-156</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t xml:space="preserve">  Net Income</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>net_income</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1,195</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>1,445</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1,711</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>2,003</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2,359</t>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>1,525</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>1,850</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2,116</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2,429</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2,799</t>
         </is>
       </c>
     </row>

</xml_diff>